<commit_message>
data set processing fix
value R/NA changed in the excel table R, I (D) was not being processed
</commit_message>
<xml_diff>
--- a/Data/US_Senate_election_data.xlsx
+++ b/Data/US_Senate_election_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matas\Google Drive\UMD\Research\senate data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A2335D-5377-4D47-AC97-2AC1199CBAF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A08D6C-7E32-49F9-90BD-9793958E2A48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{2AE6488E-656F-464F-A433-C35F6F71FD93}"/>
   </bookViews>
@@ -18,9 +18,11 @@
     <sheet name="List2" sheetId="6" r:id="rId3"/>
     <sheet name="List4" sheetId="8" r:id="rId4"/>
     <sheet name="Final" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">List4!$A$1:$CY$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Sheet1!$K$15:$K$131</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -2724,8 +2726,75 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jan Matas</author>
+  </authors>
+  <commentList>
+    <comment ref="X4" authorId="0" shapeId="0" xr:uid="{4965D2C6-5DA8-403B-B6B2-ECE81DA34C08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Independent, caucases with Dems</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{3A27D6B8-E428-4539-B36F-1746082AB23D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://en.wikipedia.org/wiki/Harry_F._Byrd_Jr.
+Independent Democrat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U11" authorId="0" shapeId="0" xr:uid="{758DD7EC-80BD-41EA-972C-1D48D36FFE50}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Independent democratic</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{CBCF6525-ABC1-4A14-8925-E5AF7F107488}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Conservative</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13580" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13706" uniqueCount="624">
   <si>
     <t>State</t>
   </si>
@@ -4594,6 +4663,9 @@
   </si>
   <si>
     <t>in 1966, only states of class II elect new senators, in 1968 only class III, etc.</t>
+  </si>
+  <si>
+    <t>data</t>
   </si>
 </sst>
 </file>
@@ -4648,7 +4720,532 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="280">
+  <dxfs count="355">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF9954CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFA86ED4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7979"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6928,8 +7525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0385F0AD-91A9-4A86-B923-9A621DDFF973}">
   <dimension ref="A1:AJ104"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="E76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O100" sqref="O100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11302,7 +11899,7 @@
         <v>53</v>
       </c>
       <c r="H47" t="s">
-        <v>428</v>
+        <v>221</v>
       </c>
       <c r="I47" t="s">
         <v>221</v>
@@ -16726,216 +17323,216 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="K3:K52 W44:Y45 Y3:Y43 W48:Y49 X46:Y47 N49:V49 AA3:AI49 AA51:AI52">
-    <cfRule type="containsText" dxfId="279" priority="402" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="354" priority="402" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="278" priority="403" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="353" priority="403" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ3:AJ9 AJ11:AJ49">
-    <cfRule type="containsText" dxfId="277" priority="400" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="352" priority="400" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AJ3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="276" priority="401" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="351" priority="401" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AJ3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3:K52 W44:X45 W48:X49 X46:X47 N49:V49 AA3:AI49 AA51:AI52">
-    <cfRule type="containsText" dxfId="275" priority="399" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="350" priority="399" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="containsText" dxfId="274" priority="361" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="349" priority="361" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AJ10)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="273" priority="362" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="348" priority="362" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AJ10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ10">
-    <cfRule type="containsText" dxfId="272" priority="360" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="347" priority="360" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AJ10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:X2 W3:X39 W41:X43 X40">
-    <cfRule type="containsText" dxfId="271" priority="111" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="346" priority="111" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="270" priority="112" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="345" priority="112" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:X2 W3:X39 W41:X43 X40">
-    <cfRule type="containsText" dxfId="269" priority="110" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="344" priority="110" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:X2 W3:X39 W41:X43 X40 N49:V49 AA3:AI49 AA51:AI52">
-    <cfRule type="containsText" dxfId="268" priority="109" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="343" priority="109" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J52">
-    <cfRule type="containsText" dxfId="267" priority="95" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="342" priority="95" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="266" priority="96" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="341" priority="96" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J52">
-    <cfRule type="containsText" dxfId="265" priority="94" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="340" priority="94" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:J52">
-    <cfRule type="containsText" dxfId="264" priority="93" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="339" priority="93" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:V39 N41:V45 N48:V50 W50 N52:W52">
-    <cfRule type="containsText" dxfId="263" priority="91" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="338" priority="91" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="262" priority="92" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="337" priority="92" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:V39 N41:V45 N48:V50 W50 N52:W52">
-    <cfRule type="containsText" dxfId="261" priority="90" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="336" priority="90" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:V39 N41:V45 N48:V50 W50 N52:W52">
-    <cfRule type="containsText" dxfId="260" priority="89" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="335" priority="89" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40">
-    <cfRule type="containsText" dxfId="259" priority="87" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="334" priority="87" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",W40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="258" priority="88" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="333" priority="88" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",W40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40">
-    <cfRule type="containsText" dxfId="257" priority="86" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="332" priority="86" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",W40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W40">
-    <cfRule type="containsText" dxfId="256" priority="85" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="331" priority="85" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",W40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:V40">
-    <cfRule type="containsText" dxfId="255" priority="83" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="330" priority="83" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="254" priority="84" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="329" priority="84" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:V40">
-    <cfRule type="containsText" dxfId="253" priority="82" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="328" priority="82" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40:V40">
-    <cfRule type="containsText" dxfId="252" priority="81" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="327" priority="81" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="containsText" dxfId="251" priority="47" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="326" priority="47" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",W46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="250" priority="48" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="325" priority="48" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",W46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="containsText" dxfId="249" priority="46" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="324" priority="46" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",W46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46">
-    <cfRule type="containsText" dxfId="248" priority="45" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="323" priority="45" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",W46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46:V46">
-    <cfRule type="containsText" dxfId="247" priority="43" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="322" priority="43" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="246" priority="44" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="321" priority="44" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46:V46">
-    <cfRule type="containsText" dxfId="245" priority="42" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="320" priority="42" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N46:V46">
-    <cfRule type="containsText" dxfId="244" priority="41" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="319" priority="41" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W47">
-    <cfRule type="containsText" dxfId="243" priority="23" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="318" priority="23" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",W47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="242" priority="24" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="317" priority="24" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",W47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W47">
-    <cfRule type="containsText" dxfId="241" priority="22" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="316" priority="22" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",W47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W47">
-    <cfRule type="containsText" dxfId="240" priority="21" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="315" priority="21" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",W47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N47:V47">
-    <cfRule type="containsText" dxfId="239" priority="19" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="314" priority="19" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="238" priority="20" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="313" priority="20" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N47:V47">
-    <cfRule type="containsText" dxfId="237" priority="18" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="312" priority="18" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N47:V47">
-    <cfRule type="containsText" dxfId="236" priority="17" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="311" priority="17" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA104:AI104">
-    <cfRule type="containsText" dxfId="235" priority="3" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="310" priority="3" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AA104)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="234" priority="4" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="309" priority="4" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AA104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA104:AI104">
-    <cfRule type="containsText" dxfId="233" priority="2" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="308" priority="2" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AA104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA104:AI104">
-    <cfRule type="containsText" dxfId="232" priority="1" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="307" priority="1" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AA104)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16950,7 +17547,7 @@
   <dimension ref="E5:M57"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H8" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17876,164 +18473,164 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F8:H57">
-    <cfRule type="containsText" dxfId="231" priority="35" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="306" priority="35" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",F8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="230" priority="36" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="305" priority="36" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:H57">
-    <cfRule type="containsText" dxfId="229" priority="34" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="304" priority="34" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8:H57">
-    <cfRule type="containsText" dxfId="228" priority="33" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="303" priority="33" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",F8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="227" priority="31" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="302" priority="31" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",G54)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="226" priority="32" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="301" priority="32" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",G54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="225" priority="30" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="300" priority="30" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",G54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G54">
-    <cfRule type="containsText" dxfId="224" priority="29" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="299" priority="29" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",G54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G44 G46:G50 G53:G55 G57">
-    <cfRule type="containsText" dxfId="223" priority="27" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="298" priority="27" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",G8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="222" priority="28" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="297" priority="28" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G44 G46:G50 G53:G55 G57">
-    <cfRule type="containsText" dxfId="221" priority="26" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="296" priority="26" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G44 G46:G50 G53:G55 G57">
-    <cfRule type="containsText" dxfId="220" priority="25" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="295" priority="25" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="219" priority="23" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="294" priority="23" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",G45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="218" priority="24" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="293" priority="24" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="217" priority="22" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="292" priority="22" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45">
-    <cfRule type="containsText" dxfId="216" priority="21" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="291" priority="21" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",G45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="215" priority="19" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="290" priority="19" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",G51)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="214" priority="20" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="289" priority="20" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="213" priority="18" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="288" priority="18" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51">
-    <cfRule type="containsText" dxfId="212" priority="17" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="287" priority="17" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",G51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="211" priority="15" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="286" priority="15" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",G52)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="210" priority="16" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="285" priority="16" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="209" priority="14" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="284" priority="14" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G52">
-    <cfRule type="containsText" dxfId="208" priority="13" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="283" priority="13" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",G52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H54 H56:H57">
-    <cfRule type="containsText" dxfId="207" priority="11" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="282" priority="11" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",H8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="206" priority="12" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="281" priority="12" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H54 H56:H57">
-    <cfRule type="containsText" dxfId="205" priority="10" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="280" priority="10" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H54 H56:H57">
-    <cfRule type="containsText" dxfId="204" priority="9" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="279" priority="9" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",H8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:W3">
-    <cfRule type="containsText" dxfId="203" priority="7" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="278" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",N3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="202" priority="8" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="277" priority="8" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:W3">
-    <cfRule type="containsText" dxfId="201" priority="6" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="276" priority="6" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N3:W3">
-    <cfRule type="containsText" dxfId="200" priority="5" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="275" priority="5" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",N3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L26">
-    <cfRule type="containsText" dxfId="199" priority="3" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="274" priority="3" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",L17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="198" priority="4" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="273" priority="4" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",L17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L26">
-    <cfRule type="containsText" dxfId="197" priority="2" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="272" priority="2" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",L17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:L26">
-    <cfRule type="containsText" dxfId="196" priority="1" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="271" priority="1" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",L17)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27156,195 +27753,195 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="T43:T44 T47:T48 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="195" priority="42" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="270" priority="42" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="194" priority="43" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="269" priority="43" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43:T44 T47:T48 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="193" priority="41" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="268" priority="41" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42">
-    <cfRule type="containsText" dxfId="192" priority="39" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="267" priority="39" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="40" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="266" priority="40" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42">
-    <cfRule type="containsText" dxfId="190" priority="38" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="265" priority="38" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="189" priority="37" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="264" priority="37" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="188" priority="35" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="263" priority="35" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="187" priority="36" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="262" priority="36" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="186" priority="34" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="261" priority="34" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="185" priority="33" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="260" priority="33" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="184" priority="31" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="259" priority="31" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="183" priority="32" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="258" priority="32" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="182" priority="30" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="257" priority="30" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="181" priority="29" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="256" priority="29" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="180" priority="27" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="255" priority="27" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="28" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="254" priority="28" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="178" priority="26" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="253" priority="26" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="177" priority="25" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="252" priority="25" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="176" priority="23" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="251" priority="23" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="175" priority="24" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="250" priority="24" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="174" priority="22" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="249" priority="22" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="173" priority="21" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="248" priority="21" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="172" priority="19" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="247" priority="19" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="171" priority="20" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="246" priority="20" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="170" priority="18" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="245" priority="18" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="169" priority="17" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="244" priority="17" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="168" priority="15" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="243" priority="15" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="16" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="242" priority="16" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="166" priority="14" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="241" priority="14" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="165" priority="13" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="240" priority="13" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="164" priority="11" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="239" priority="11" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="163" priority="12" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="238" priority="12" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="162" priority="10" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="237" priority="10" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="161" priority="9" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="236" priority="9" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="160" priority="7" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="235" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="8" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="234" priority="8" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="158" priority="6" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="233" priority="6" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="157" priority="5" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="232" priority="5" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U103:AC103">
-    <cfRule type="containsText" dxfId="156" priority="3" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="231" priority="3" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",U103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="155" priority="4" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="230" priority="4" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",U103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U103:AC103">
-    <cfRule type="containsText" dxfId="154" priority="2" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="229" priority="2" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",U103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U103:AC103">
-    <cfRule type="containsText" dxfId="153" priority="1" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="228" priority="1" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",U103)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46148,352 +46745,352 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="AQ20:AR20 AU20:AV20 AV11:AV19 B21:AV29 AX21:AY29">
-    <cfRule type="containsText" dxfId="152" priority="81" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="227" priority="81" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="151" priority="82" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="226" priority="82" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ20:AR20 AU20:AV20 AV11:AV19 B21:AV29 AX21:AY29">
-    <cfRule type="containsText" dxfId="150" priority="80" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="225" priority="80" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A20 B20:AL20 AN20:AP20">
-    <cfRule type="containsText" dxfId="149" priority="78" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="224" priority="78" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",A11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="148" priority="79" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="223" priority="79" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A20 B20:AL20 AN20:AP20">
-    <cfRule type="containsText" dxfId="147" priority="77" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="222" priority="77" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A20 B20:AL20 AN20:AP20 AV11:AV19 B21:AV29 AX21:AY29">
-    <cfRule type="containsText" dxfId="146" priority="76" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="221" priority="76" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",A11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AY10">
-    <cfRule type="containsText" dxfId="145" priority="74" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="220" priority="74" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="144" priority="75" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="219" priority="75" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AY10">
-    <cfRule type="containsText" dxfId="143" priority="73" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="218" priority="73" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:AY10">
-    <cfRule type="containsText" dxfId="142" priority="72" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="217" priority="72" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:AL19 AN11:AR19 AU11:AW19 AW20 AY11:AY20">
-    <cfRule type="containsText" dxfId="141" priority="70" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="216" priority="70" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="71" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="215" priority="71" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:AL19 AN11:AR19 AU11:AW19 AW20 AY11:AY20">
-    <cfRule type="containsText" dxfId="139" priority="69" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="214" priority="69" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:AL19 AN11:AR19 AU11:AW19 AW20 AY11:AY20">
-    <cfRule type="containsText" dxfId="138" priority="68" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="213" priority="68" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM20">
-    <cfRule type="containsText" dxfId="137" priority="66" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="212" priority="66" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AM20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="67" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="211" priority="67" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AM20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM20">
-    <cfRule type="containsText" dxfId="135" priority="65" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="210" priority="65" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AM20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM20">
-    <cfRule type="containsText" dxfId="134" priority="64" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="209" priority="64" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AM20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM11:AM19">
-    <cfRule type="containsText" dxfId="133" priority="62" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="208" priority="62" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AM11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="63" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="207" priority="63" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AM11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM11:AM19">
-    <cfRule type="containsText" dxfId="131" priority="61" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="206" priority="61" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AM11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM11:AM19">
-    <cfRule type="containsText" dxfId="130" priority="60" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="205" priority="60" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AM11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS20">
-    <cfRule type="containsText" dxfId="129" priority="58" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="204" priority="58" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AS20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="59" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="203" priority="59" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AS20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS20">
-    <cfRule type="containsText" dxfId="127" priority="57" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="202" priority="57" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AS20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS20">
-    <cfRule type="containsText" dxfId="126" priority="56" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="201" priority="56" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AS20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS11:AS19">
-    <cfRule type="containsText" dxfId="125" priority="54" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="200" priority="54" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AS11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="55" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="199" priority="55" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AS11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS11:AS19">
-    <cfRule type="containsText" dxfId="123" priority="53" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="198" priority="53" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AS11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS11:AS19">
-    <cfRule type="containsText" dxfId="122" priority="52" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="197" priority="52" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AS11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT20">
-    <cfRule type="containsText" dxfId="121" priority="50" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="196" priority="50" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AT20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="51" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="195" priority="51" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AT20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT20">
-    <cfRule type="containsText" dxfId="119" priority="49" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="194" priority="49" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AT20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT20">
-    <cfRule type="containsText" dxfId="118" priority="48" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="193" priority="48" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AT20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT11:AT19">
-    <cfRule type="containsText" dxfId="117" priority="46" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="192" priority="46" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AT11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="47" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="191" priority="47" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AT11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT11:AT19">
-    <cfRule type="containsText" dxfId="115" priority="45" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="190" priority="45" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AT11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT11:AT19">
-    <cfRule type="containsText" dxfId="114" priority="44" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="189" priority="44" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AT11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:S77">
-    <cfRule type="containsText" dxfId="113" priority="3" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="188" priority="3" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="4" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="187" priority="4" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:S77">
-    <cfRule type="containsText" dxfId="111" priority="2" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="186" priority="2" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K77:S77">
-    <cfRule type="containsText" dxfId="110" priority="1" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="185" priority="1" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T74:T75 T78:T79 K79:S79 U33:AC79 U81:AC85">
-    <cfRule type="containsText" dxfId="109" priority="38" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="184" priority="38" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="39" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="183" priority="39" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T74:T75 T78:T79 K79:S79 U33:AC79 U81:AC85">
-    <cfRule type="containsText" dxfId="107" priority="37" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="182" priority="37" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:T32 T33:T69 T71:T73">
-    <cfRule type="containsText" dxfId="106" priority="35" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="181" priority="35" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K32)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="36" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="180" priority="36" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:T32 T33:T69 T71:T73">
-    <cfRule type="containsText" dxfId="104" priority="34" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="179" priority="34" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:T32 T33:T69 T71:T73 K79:S79 U33:AC79 U81:AC85">
-    <cfRule type="containsText" dxfId="103" priority="33" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="178" priority="33" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:J85">
-    <cfRule type="containsText" dxfId="102" priority="31" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="177" priority="31" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="32" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="176" priority="32" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:J85">
-    <cfRule type="containsText" dxfId="100" priority="30" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="175" priority="30" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:J85">
-    <cfRule type="containsText" dxfId="99" priority="29" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="174" priority="29" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:S69 K71:S75 K78:S80 T80 K82:T85">
-    <cfRule type="containsText" dxfId="98" priority="27" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="173" priority="27" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K33)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="28" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="172" priority="28" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:S69 K71:S75 K78:S80 T80 K82:T85">
-    <cfRule type="containsText" dxfId="96" priority="26" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="171" priority="26" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:S69 K71:S75 K78:S80 T80 K82:T85">
-    <cfRule type="containsText" dxfId="95" priority="25" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="170" priority="25" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T70">
-    <cfRule type="containsText" dxfId="94" priority="23" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="169" priority="23" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="24" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="168" priority="24" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T70">
-    <cfRule type="containsText" dxfId="92" priority="22" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="167" priority="22" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T70">
-    <cfRule type="containsText" dxfId="91" priority="21" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="166" priority="21" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:S70">
-    <cfRule type="containsText" dxfId="90" priority="19" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="165" priority="19" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K70)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="20" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="164" priority="20" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:S70">
-    <cfRule type="containsText" dxfId="88" priority="18" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="163" priority="18" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:S70">
-    <cfRule type="containsText" dxfId="87" priority="17" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="162" priority="17" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K70)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T76">
-    <cfRule type="containsText" dxfId="86" priority="15" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="161" priority="15" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="16" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="160" priority="16" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T76">
-    <cfRule type="containsText" dxfId="84" priority="14" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="159" priority="14" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T76">
-    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="158" priority="13" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76:S76">
-    <cfRule type="containsText" dxfId="82" priority="11" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="157" priority="11" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="12" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="156" priority="12" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76:S76">
-    <cfRule type="containsText" dxfId="80" priority="10" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="155" priority="10" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K76:S76">
-    <cfRule type="containsText" dxfId="79" priority="9" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="154" priority="9" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T77">
-    <cfRule type="containsText" dxfId="78" priority="7" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="153" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T77)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="8" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="152" priority="8" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T77">
-    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="151" priority="6" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T77)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T77">
-    <cfRule type="containsText" dxfId="75" priority="5" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="150" priority="5" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T77)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46507,8 +47104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{494DAB8E-C38B-4181-8A5B-0071F0B07073}">
   <dimension ref="A1:AD51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47513,7 +48110,7 @@
         <v>53</v>
       </c>
       <c r="AA11" t="s">
-        <v>149</v>
+        <v>53</v>
       </c>
       <c r="AB11" t="s">
         <v>80</v>
@@ -50718,7 +51315,7 @@
         <v>52</v>
       </c>
       <c r="V46" t="s">
-        <v>428</v>
+        <v>221</v>
       </c>
       <c r="W46" t="s">
         <v>80</v>
@@ -51207,343 +51804,841 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="74" priority="39" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="149" priority="39" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="40" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="148" priority="40" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="72" priority="38" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="147" priority="38" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:S46">
-    <cfRule type="containsText" dxfId="71" priority="37" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="146" priority="37" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43:T44 T47:T48 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="145" priority="74" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="144" priority="75" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T43:T44 T47:T48 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="68" priority="73" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="143" priority="73" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42">
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="142" priority="71" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="141" priority="72" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42">
-    <cfRule type="containsText" dxfId="65" priority="70" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="140" priority="70" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:T1 T2:T38 T40:T42 K48:S48 U2:AC48 U50:AC51">
-    <cfRule type="containsText" dxfId="64" priority="69" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="139" priority="69" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="138" priority="67" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="68" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="137" priority="68" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="61" priority="66" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="136" priority="66" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:J51">
-    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="135" priority="65" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="134" priority="63" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="64" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="133" priority="64" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="132" priority="62" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:S38 K40:S44 K47:S49 T49 K51:T51">
-    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="131" priority="61" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="130" priority="59" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="60" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="129" priority="60" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="53" priority="58" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="128" priority="58" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T39">
-    <cfRule type="containsText" dxfId="52" priority="57" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="127" priority="57" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="126" priority="55" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K39)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="56" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="125" priority="56" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="49" priority="54" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="124" priority="54" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:S39">
-    <cfRule type="containsText" dxfId="48" priority="53" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="123" priority="53" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="47" priority="51" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="122" priority="51" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="52" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="121" priority="52" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="120" priority="50" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="containsText" dxfId="44" priority="49" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="119" priority="49" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="118" priority="47" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",K45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="48" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="117" priority="48" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="41" priority="46" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="116" priority="46" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:S45">
-    <cfRule type="containsText" dxfId="40" priority="45" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="115" priority="45" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",K45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="114" priority="43" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",T46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="44" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="113" priority="44" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="112" priority="42" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T46">
-    <cfRule type="containsText" dxfId="36" priority="41" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="111" priority="41" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",T46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB49">
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="110" priority="35" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AB49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="36" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="109" priority="36" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AB49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB49">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="108" priority="34" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AB49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB49">
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="107" priority="33" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AB49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="106" priority="31" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",Y49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="105" priority="32" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",Y49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49">
-    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="104" priority="30" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",Y49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y49">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="103" priority="29" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",Y49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V49:W49">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="102" priority="27" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",V49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="101" priority="28" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",V49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V49:W49">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="100" priority="26" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",V49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V49:W49">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="99" priority="25" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",V49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="98" priority="23" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",AC49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="97" priority="24" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",AC49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="96" priority="22" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",AC49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="95" priority="21" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",AC49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z49">
-    <cfRule type="containsText" dxfId="19" priority="19" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="94" priority="19" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",Z49)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="20" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="93" priority="20" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",Z49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z49">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",Z49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z49">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="91" priority="17" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",Z49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="90" priority="15" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",L50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="16" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="89" priority="16" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",L50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="88" priority="14" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",L50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="87" priority="13" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",L50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="86" priority="11" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",M50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="85" priority="12" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",M50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="84" priority="10" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",M50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M50">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="83" priority="9" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",M50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50:P50">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="82" priority="7" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",O50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="81" priority="8" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",O50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50:P50">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="80" priority="6" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",O50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O50:P50">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="79" priority="5" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",O50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R50:S50">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="R">
+    <cfRule type="containsText" dxfId="78" priority="3" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",R50)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="D">
+    <cfRule type="containsText" dxfId="77" priority="4" operator="containsText" text="D">
       <formula>NOT(ISERROR(SEARCH("D",R50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R50:S50">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="R/D">
+    <cfRule type="containsText" dxfId="76" priority="2" operator="containsText" text="R/D">
       <formula>NOT(ISERROR(SEARCH("R/D",R50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R50:S50">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="D/R">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="D/R">
       <formula>NOT(ISERROR(SEARCH("D/R",R50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9523F4DF-3EAF-48EC-AE7A-1F4998B96BA6}">
+  <dimension ref="A1:AB34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P1" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U1" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" t="s">
+        <v>52</v>
+      </c>
+      <c r="W2" t="s">
+        <v>52</v>
+      </c>
+      <c r="X2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J3" t="s">
+        <v>80</v>
+      </c>
+      <c r="K3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" t="s">
+        <v>80</v>
+      </c>
+      <c r="U3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V3" t="s">
+        <v>80</v>
+      </c>
+      <c r="W3" t="s">
+        <v>80</v>
+      </c>
+      <c r="X3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>233</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
+        <v>233</v>
+      </c>
+      <c r="K4" t="s">
+        <v>181</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>233</v>
+      </c>
+      <c r="N4" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>59</v>
+      </c>
+      <c r="R4" t="s">
+        <v>233</v>
+      </c>
+      <c r="U4" t="s">
+        <v>233</v>
+      </c>
+      <c r="V4" t="s">
+        <v>241</v>
+      </c>
+      <c r="W4" t="s">
+        <v>241</v>
+      </c>
+      <c r="X4" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="F5" t="s">
+        <v>221</v>
+      </c>
+      <c r="L5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N5" t="s">
+        <v>59</v>
+      </c>
+      <c r="U5" t="s">
+        <v>181</v>
+      </c>
+      <c r="W5" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>233</v>
+      </c>
+      <c r="U6" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="U7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="K15" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K22" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K23" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <autoFilter ref="K15:K131" xr:uid="{0709B11A-912C-434F-95C1-2976DCC86448}"/>
+  <conditionalFormatting sqref="T1:AB3 U4:AA4 U5:U7 W5 Y5:Z5 Y6">
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",T1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="69" priority="75" operator="containsText" text="D">
+      <formula>NOT(ISERROR(SEARCH("D",T1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T1:AB3 U4:AA4 U5:U7 W5 Y5:Z5 Y6">
+    <cfRule type="containsText" dxfId="68" priority="73" operator="containsText" text="R/D">
+      <formula>NOT(ISERROR(SEARCH("R/D",T1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S3">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",S1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="72" operator="containsText" text="D">
+      <formula>NOT(ISERROR(SEARCH("D",S1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:S3">
+    <cfRule type="containsText" dxfId="65" priority="70" operator="containsText" text="R/D">
+      <formula>NOT(ISERROR(SEARCH("R/D",S1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="S1:AB3 U4:AA4 U5:U7 W5 Y5:Z5 Y6">
+    <cfRule type="containsText" dxfId="64" priority="69" operator="containsText" text="D/R">
+      <formula>NOT(ISERROR(SEARCH("D/R",S1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I3 C5 A4:C4 E4:F4 F5 H4:I4">
+    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="68" operator="containsText" text="D">
+      <formula>NOT(ISERROR(SEARCH("D",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I3 C5 A4:C4 E4:F4 F5 H4:I4">
+    <cfRule type="containsText" dxfId="61" priority="66" operator="containsText" text="R/D">
+      <formula>NOT(ISERROR(SEARCH("R/D",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:I3 C5 A4:C4 E4:F4 F5 H4:I4">
+    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="D/R">
+      <formula>NOT(ISERROR(SEARCH("D/R",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:R3 K4:N4 L5:L6 N5 Q4:R4">
+    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="58" priority="64" operator="containsText" text="D">
+      <formula>NOT(ISERROR(SEARCH("D",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:R3 K4:N4 L5:L6 N5 Q4:R4">
+    <cfRule type="containsText" dxfId="57" priority="62" operator="containsText" text="R/D">
+      <formula>NOT(ISERROR(SEARCH("R/D",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:R3 K4:N4 L5:L6 N5 Q4:R4">
+    <cfRule type="containsText" dxfId="56" priority="61" operator="containsText" text="D/R">
+      <formula>NOT(ISERROR(SEARCH("D/R",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>